<commit_message>
make all booleans start with is_
</commit_message>
<xml_diff>
--- a/a_in/us_travels.xlsx
+++ b/a_in/us_travels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s9/Code/us_travels_v4/a_in/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E116E6-C5CD-754F-8801-9AB273AF0327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9119BC74-EDA9-D540-9320-3CE71ADDA13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53640" yWindow="640" windowWidth="18120" windowHeight="20960" firstSheet="2" activeTab="7" xr2:uid="{895BEAD3-490B-3645-811C-E95312094DBD}"/>
+    <workbookView xWindow="53640" yWindow="640" windowWidth="18120" windowHeight="20960" firstSheet="2" activeTab="2" xr2:uid="{895BEAD3-490B-3645-811C-E95312094DBD}"/>
   </bookViews>
   <sheets>
     <sheet name="msa_roster" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3541" uniqueCount="1190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3540" uniqueCount="1189">
   <si>
     <t>New York–Newark–Jersey City, NY-NJ MSA</t>
   </si>
@@ -3479,9 +3479,6 @@
     <t>Mega City</t>
   </si>
   <si>
-    <t>goal</t>
-  </si>
-  <si>
     <t>UVA / Montecello WHS</t>
   </si>
   <si>
@@ -3596,9 +3593,6 @@
     <t>Ocean City MD</t>
   </si>
   <si>
-    <t>trips</t>
-  </si>
-  <si>
     <t>2021-Virginia</t>
   </si>
   <si>
@@ -3615,6 +3609,9 @@
   </si>
   <si>
     <t>visit</t>
+  </si>
+  <si>
+    <t>is_goal</t>
   </si>
 </sst>
 </file>
@@ -4098,17 +4095,17 @@
   <dimension ref="A1:L397"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C215" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E249" sqref="E249"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.83203125" style="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="12" customWidth="1"/>
     <col min="6" max="6" width="13.1640625" style="13" bestFit="1" customWidth="1"/>
@@ -4127,10 +4124,10 @@
         <v>587</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>1144</v>
+        <v>1188</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>1142</v>
@@ -4542,7 +4539,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="B13" t="s">
         <v>589</v>
@@ -5809,7 +5806,7 @@
       <c r="F48" s="11"/>
       <c r="G48" s="11"/>
       <c r="H48" s="11" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="I48" s="10">
         <v>156840</v>
@@ -6564,7 +6561,7 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="B70" t="s">
         <v>703</v>
@@ -6578,13 +6575,13 @@
         <v>1</v>
       </c>
       <c r="H70" s="13" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="I70" s="12">
         <v>93875</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="K70" t="s">
         <v>17</v>
@@ -7982,7 +7979,7 @@
       <c r="F109" s="11"/>
       <c r="G109" s="11"/>
       <c r="H109" s="11" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="I109" s="10">
         <v>227336</v>
@@ -17487,10 +17484,10 @@
   <dimension ref="A1:H86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E89" sqref="E89"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17504,7 +17501,7 @@
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>839</v>
       </c>
@@ -17523,11 +17520,8 @@
       <c r="F1" t="s">
         <v>933</v>
       </c>
-      <c r="G1" t="s">
-        <v>1183</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>838</v>
       </c>
@@ -17548,7 +17542,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>838</v>
       </c>
@@ -17569,7 +17563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>842</v>
       </c>
@@ -17590,7 +17584,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>842</v>
       </c>
@@ -17611,7 +17605,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>842</v>
       </c>
@@ -17632,7 +17626,7 @@
         <v>31.1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>841</v>
       </c>
@@ -17653,7 +17647,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>843</v>
       </c>
@@ -17674,7 +17668,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>843</v>
       </c>
@@ -17695,7 +17689,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>838</v>
       </c>
@@ -17716,7 +17710,7 @@
         <v>99.9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>838</v>
       </c>
@@ -17737,7 +17731,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>838</v>
       </c>
@@ -17758,7 +17752,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>838</v>
       </c>
@@ -17779,7 +17773,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>838</v>
       </c>
@@ -17800,7 +17794,7 @@
         <v>14.3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>838</v>
       </c>
@@ -17821,7 +17815,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>838</v>
       </c>
@@ -19332,11 +19326,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A1812C-866A-0544-AE9F-235DC4187F8D}">
   <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F32" sqref="F32"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21195,18 +21189,18 @@
         <v>1140</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="B2" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C2" s="20">
         <f>DATE(2014,6,15)</f>
@@ -21219,10 +21213,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="B3" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="C3" s="18">
         <f>DATE(2016,12,23)</f>
@@ -21235,10 +21229,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="B4" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="C4" s="20">
         <f>DATE(2017,6,15)</f>
@@ -21251,10 +21245,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B5" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="C5" s="18">
         <f>DATE(2021,5,10)</f>
@@ -21267,10 +21261,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="B6" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="C6" s="4">
         <f>DATE(2021,6,7)</f>
@@ -21283,10 +21277,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B7" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="C7" s="19">
         <f>DATE(2021,8,31)</f>
@@ -21300,10 +21294,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="B8" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="C8" s="4">
         <f>DATE(2021,10,9)</f>
@@ -21317,10 +21311,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B9" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="C9" s="18">
         <f>DATE(2021,10,18)</f>
@@ -21333,10 +21327,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="B10" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="C10" s="4">
         <f>DATE(2023,8,25)</f>
@@ -21349,10 +21343,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B11" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="C11" s="18">
         <f>DATE(2022,8,21)</f>
@@ -21365,10 +21359,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="B12" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="C12" s="4">
         <f>DATE(2022,9,24)</f>
@@ -21381,10 +21375,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B13" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="C13" s="18">
         <f>DATE(2023,5,12)</f>
@@ -21397,10 +21391,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B14" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="C14" s="18">
         <f>DATE(2023,12,14)</f>
@@ -21413,10 +21407,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B15" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="C15" s="18">
         <f>DATE(2024,9,17)</f>
@@ -21459,12 +21453,12 @@
         <v>1139</v>
       </c>
       <c r="B1" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>681</v>
@@ -21472,7 +21466,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="B3" t="s">
         <v>648</v>
@@ -21480,7 +21474,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="B4" t="s">
         <v>557</v>
@@ -21488,7 +21482,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="B5" t="s">
         <v>553</v>
@@ -21496,7 +21490,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="B6" t="s">
         <v>683</v>
@@ -21504,7 +21498,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>551</v>
@@ -21512,7 +21506,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>551</v>
@@ -21520,7 +21514,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="B9" t="s">
         <v>861</v>
@@ -21528,7 +21522,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="B10" t="s">
         <v>575</v>
@@ -21536,7 +21530,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="B11" t="s">
         <v>576</v>
@@ -21544,7 +21538,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="B12" t="s">
         <v>564</v>
@@ -21552,7 +21546,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>551</v>
@@ -21560,7 +21554,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="B14" t="s">
         <v>574</v>
@@ -21568,7 +21562,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="B15" t="s">
         <v>681</v>
@@ -21576,7 +21570,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="B16" t="s">
         <v>656</v>
@@ -21584,7 +21578,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="B17" t="s">
         <v>554</v>
@@ -21592,7 +21586,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="B18" t="s">
         <v>644</v>
@@ -21600,7 +21594,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="B19" t="s">
         <v>559</v>
@@ -21608,7 +21602,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="B20" t="s">
         <v>599</v>
@@ -21616,7 +21610,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="B21" t="s">
         <v>573</v>
@@ -21624,7 +21618,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="B22" t="s">
         <v>865</v>
@@ -21632,7 +21626,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="B23" t="s">
         <v>709</v>
@@ -21640,7 +21634,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="21" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B24" s="21" t="s">
         <v>556</v>
@@ -21648,7 +21642,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B25" t="s">
         <v>560</v>
@@ -21656,7 +21650,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B26" t="s">
         <v>746</v>
@@ -21664,7 +21658,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B27" t="s">
         <v>631</v>
@@ -21672,15 +21666,15 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B28" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="21" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B29" s="21" t="s">
         <v>556</v>
@@ -21688,7 +21682,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B30" t="s">
         <v>721</v>
@@ -21696,7 +21690,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B31" t="s">
         <v>579</v>
@@ -21704,7 +21698,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B32" t="s">
         <v>1102</v>
@@ -21712,7 +21706,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B33" t="s">
         <v>581</v>
@@ -21720,7 +21714,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B34" t="s">
         <v>669</v>
@@ -21728,7 +21722,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B35" t="s">
         <v>739</v>
@@ -21736,7 +21730,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B36" t="s">
         <v>582</v>
@@ -21744,7 +21738,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B37" t="s">
         <v>727</v>
@@ -21752,7 +21746,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B38" t="s">
         <v>580</v>
@@ -21760,7 +21754,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B39" t="s">
         <v>707</v>
@@ -21768,7 +21762,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B40" t="s">
         <v>598</v>
@@ -21776,7 +21770,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B41" t="s">
         <v>897</v>
@@ -21784,7 +21778,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B42" t="s">
         <v>637</v>
@@ -21792,7 +21786,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B43" t="s">
         <v>720</v>
@@ -21800,7 +21794,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B44" t="s">
         <v>572</v>
@@ -21808,7 +21802,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B45" t="s">
         <v>717</v>
@@ -21816,7 +21810,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="21" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B46" s="21" t="s">
         <v>556</v>
@@ -21824,7 +21818,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B47" t="s">
         <v>652</v>
@@ -21832,7 +21826,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B48" t="s">
         <v>879</v>
@@ -21840,7 +21834,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B49" t="s">
         <v>560</v>
@@ -21848,7 +21842,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B50" t="s">
         <v>633</v>
@@ -21856,7 +21850,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B51" t="s">
         <v>719</v>
@@ -21864,7 +21858,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B52" t="s">
         <v>682</v>
@@ -21872,7 +21866,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B53" t="s">
         <v>700</v>
@@ -21880,7 +21874,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B54" t="s">
         <v>751</v>
@@ -21888,7 +21882,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B55" t="s">
         <v>689</v>
@@ -21896,7 +21890,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B56" t="s">
         <v>692</v>
@@ -21904,7 +21898,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B57" t="s">
         <v>594</v>
@@ -21912,7 +21906,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B58" t="s">
         <v>636</v>
@@ -21920,7 +21914,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B59" t="s">
         <v>704</v>
@@ -21928,7 +21922,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B60" t="s">
         <v>885</v>
@@ -21936,7 +21930,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="21" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="B61" s="21" t="s">
         <v>551</v>
@@ -21944,7 +21938,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="B62" t="s">
         <v>578</v>
@@ -21952,7 +21946,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="B63" t="s">
         <v>561</v>
@@ -21960,7 +21954,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="B64" t="s">
         <v>567</v>
@@ -21968,7 +21962,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="21" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="B65" s="21" t="s">
         <v>556</v>
@@ -21976,7 +21970,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="B66" t="s">
         <v>858</v>
@@ -21984,7 +21978,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="B67" t="s">
         <v>681</v>
@@ -21992,7 +21986,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="B68" t="s">
         <v>599</v>
@@ -22000,7 +21994,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="21" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B69" s="21" t="s">
         <v>556</v>
@@ -22008,7 +22002,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B70" t="s">
         <v>934</v>
@@ -22016,7 +22010,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B71" t="s">
         <v>552</v>
@@ -22024,7 +22018,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B72" t="s">
         <v>583</v>
@@ -22032,7 +22026,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B73" t="s">
         <v>872</v>
@@ -22040,7 +22034,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B74" t="s">
         <v>563</v>
@@ -22048,7 +22042,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B75" t="s">
         <v>630</v>
@@ -22056,7 +22050,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B76" t="s">
         <v>711</v>
@@ -22064,7 +22058,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B77" t="s">
         <v>745</v>
@@ -22072,7 +22066,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B78" t="s">
         <v>673</v>
@@ -22080,7 +22074,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B79" t="s">
         <v>595</v>
@@ -22088,7 +22082,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B80" t="s">
         <v>577</v>
@@ -22096,7 +22090,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B81" t="s">
         <v>556</v>
@@ -22104,7 +22098,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="21" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="B82" s="21" t="s">
         <v>648</v>
@@ -22112,7 +22106,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="B83" t="s">
         <v>726</v>
@@ -22120,7 +22114,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="21" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="B84" s="21" t="s">
         <v>556</v>
@@ -22128,7 +22122,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="B85" t="s">
         <v>743</v>
@@ -22136,7 +22130,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="B86" t="s">
         <v>723</v>
@@ -22144,7 +22138,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="21" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B87" s="21" t="s">
         <v>556</v>
@@ -22152,7 +22146,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B88" t="s">
         <v>681</v>
@@ -22160,7 +22154,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B89" t="s">
         <v>593</v>
@@ -22168,7 +22162,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B90" t="s">
         <v>555</v>
@@ -22176,7 +22170,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B91" t="s">
         <v>569</v>
@@ -22184,7 +22178,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B92" t="s">
         <v>599</v>
@@ -22192,7 +22186,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B93" t="s">
         <v>865</v>
@@ -22200,7 +22194,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B94" t="s">
         <v>709</v>
@@ -22208,7 +22202,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B95" t="s">
         <v>566</v>
@@ -22216,7 +22210,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="21" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B96" s="21" t="s">
         <v>556</v>
@@ -22224,7 +22218,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B97" t="s">
         <v>557</v>
@@ -22232,7 +22226,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B98" t="s">
         <v>602</v>
@@ -22240,7 +22234,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B99" t="s">
         <v>658</v>
@@ -22248,7 +22242,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B100" t="s">
         <v>570</v>
@@ -22256,7 +22250,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B101" t="s">
         <v>657</v>
@@ -22264,7 +22258,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B102" t="s">
         <v>681</v>
@@ -22272,7 +22266,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B103" t="s">
         <v>646</v>
@@ -22280,7 +22274,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B104" t="s">
         <v>708</v>
@@ -22288,7 +22282,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B105" t="s">
         <v>584</v>
@@ -22296,7 +22290,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B106" t="s">
         <v>599</v>
@@ -22304,7 +22298,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B107" t="s">
         <v>865</v>
@@ -22312,7 +22306,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B108" t="s">
         <v>592</v>
@@ -22320,7 +22314,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="21" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B109" s="21" t="s">
         <v>556</v>
@@ -22328,7 +22322,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B110" t="s">
         <v>728</v>
@@ -22336,7 +22330,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B111" t="s">
         <v>716</v>
@@ -22344,7 +22338,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B112" t="s">
         <v>673</v>
@@ -22352,7 +22346,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B113" t="s">
         <v>595</v>
@@ -22360,7 +22354,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B114" t="s">
         <v>565</v>
@@ -22368,7 +22362,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B115" t="s">
         <v>637</v>
@@ -22376,7 +22370,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B116" t="s">
         <v>748</v>
@@ -22384,7 +22378,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B117" t="s">
         <v>859</v>
@@ -22392,7 +22386,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B118" t="s">
         <v>713</v>
@@ -22424,7 +22418,7 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="J38" sqref="J38"/>
@@ -22446,10 +22440,10 @@
         <v>1139</v>
       </c>
       <c r="B1" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C1" t="s">
         <v>1173</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1174</v>
       </c>
       <c r="D1" t="s">
         <v>1136</v>
@@ -22458,12 +22452,12 @@
         <v>1137</v>
       </c>
       <c r="F1" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B2" t="s">
         <v>556</v>
@@ -22474,7 +22468,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B3" t="s">
         <v>577</v>
@@ -22485,7 +22479,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B4" t="s">
         <v>581</v>
@@ -22496,7 +22490,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B5" t="s">
         <v>582</v>
@@ -22507,7 +22501,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B6" t="s">
         <v>552</v>
@@ -22518,7 +22512,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B7" t="s">
         <v>673</v>
@@ -22529,7 +22523,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B8" t="s">
         <v>565</v>
@@ -22540,7 +22534,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B9" t="s">
         <v>716</v>
@@ -22551,7 +22545,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B10" t="s">
         <v>728</v>
@@ -22564,12 +22558,12 @@
         <v>46.933005000000001</v>
       </c>
       <c r="F10" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B11" s="16"/>
       <c r="C11" t="s">
@@ -22578,7 +22572,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B12" t="s">
         <v>859</v>
@@ -22589,7 +22583,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B13" t="s">
         <v>748</v>
@@ -22600,7 +22594,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B14" t="s">
         <v>713</v>
@@ -22611,7 +22605,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B15" t="s">
         <v>637</v>
@@ -22622,7 +22616,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B16" t="s">
         <v>669</v>
@@ -22633,7 +22627,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B17" t="s">
         <v>582</v>
@@ -22644,7 +22638,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B18" t="s">
         <v>581</v>
@@ -22655,7 +22649,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B19" t="s">
         <v>577</v>
@@ -22666,7 +22660,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B20" t="s">
         <v>556</v>
@@ -22677,7 +22671,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B21" t="s">
         <v>599</v>
@@ -22688,7 +22682,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B22" t="s">
         <v>596</v>
@@ -22699,7 +22693,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>657</v>
@@ -22710,7 +22704,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B24" t="s">
         <v>865</v>
@@ -22721,7 +22715,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B25" t="s">
         <v>593</v>
@@ -22732,7 +22726,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B26" t="s">
         <v>569</v>
@@ -22743,7 +22737,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B27" t="s">
         <v>555</v>
@@ -22754,7 +22748,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B28" t="s">
         <v>566</v>
@@ -22765,7 +22759,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B29" t="s">
         <v>709</v>
@@ -22776,7 +22770,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B30" t="s">
         <v>593</v>
@@ -22787,7 +22781,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B31" t="s">
         <v>865</v>
@@ -22798,7 +22792,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B32" t="s">
         <v>596</v>
@@ -22809,7 +22803,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B33" t="s">
         <v>599</v>
@@ -22820,7 +22814,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="B34" t="s">
         <v>556</v>
@@ -22831,7 +22825,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="B35" t="s">
         <v>743</v>
@@ -22842,7 +22836,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="B36" t="s">
         <v>723</v>
@@ -22855,12 +22849,12 @@
         <v>38.333578000000003</v>
       </c>
       <c r="F36" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="B37" s="16"/>
       <c r="C37" t="s">
@@ -22869,7 +22863,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="B38" t="s">
         <v>743</v>
@@ -22880,7 +22874,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B39" t="s">
         <v>556</v>
@@ -22891,7 +22885,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>858</v>
@@ -22902,7 +22896,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B41" t="s">
         <v>646</v>
@@ -22913,7 +22907,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B42" t="s">
         <v>584</v>
@@ -22924,7 +22918,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B43" t="s">
         <v>602</v>
@@ -22935,7 +22929,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B44" t="s">
         <v>708</v>
@@ -22946,7 +22940,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B45" t="s">
         <v>557</v>
@@ -22957,7 +22951,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B46" t="s">
         <v>865</v>
@@ -22968,7 +22962,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B47" t="s">
         <v>658</v>
@@ -22979,7 +22973,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B48" t="s">
         <v>657</v>
@@ -22990,7 +22984,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B49" t="s">
         <v>570</v>
@@ -23001,7 +22995,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B50" s="15" t="s">
         <v>596</v>
@@ -23012,7 +23006,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B51" t="s">
         <v>592</v>
@@ -23023,7 +23017,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B52" t="s">
         <v>599</v>
@@ -23034,7 +23028,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="B53" t="s">
         <v>648</v>
@@ -23045,7 +23039,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="B54" t="s">
         <v>726</v>
@@ -23056,7 +23050,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B55" t="s">
         <v>556</v>
@@ -23067,7 +23061,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B56" t="s">
         <v>577</v>
@@ -23078,7 +23072,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B57" t="s">
         <v>583</v>
@@ -23089,7 +23083,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B58" t="s">
         <v>745</v>
@@ -23100,7 +23094,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B59" t="s">
         <v>630</v>
@@ -23111,7 +23105,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B60" t="s">
         <v>552</v>
@@ -23122,7 +23116,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B61" t="s">
         <v>673</v>
@@ -23133,7 +23127,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B62" t="s">
         <v>595</v>
@@ -23146,12 +23140,12 @@
         <v>46.412545000000001</v>
       </c>
       <c r="F62" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B63" s="16"/>
       <c r="C63" t="s">
@@ -23160,7 +23154,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B64" t="s">
         <v>563</v>
@@ -23171,7 +23165,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B65" t="s">
         <v>583</v>
@@ -23182,7 +23176,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B66" t="s">
         <v>577</v>
@@ -23193,7 +23187,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="B67" t="s">
         <v>551</v>
@@ -23204,7 +23198,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="B68" t="s">
         <v>567</v>
@@ -23215,7 +23209,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="B69" t="s">
         <v>561</v>
@@ -23226,7 +23220,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B70" t="s">
         <v>556</v>
@@ -23237,7 +23231,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B71" t="s">
         <v>577</v>
@@ -23248,7 +23242,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B72" t="s">
         <v>581</v>
@@ -23259,7 +23253,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B73" t="s">
         <v>579</v>
@@ -23270,7 +23264,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B74" t="s">
         <v>582</v>
@@ -23281,7 +23275,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B75" t="s">
         <v>720</v>
@@ -23292,7 +23286,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B76" t="s">
         <v>669</v>
@@ -23303,7 +23297,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B77" t="s">
         <v>637</v>
@@ -23314,7 +23308,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B78" t="s">
         <v>707</v>
@@ -23325,7 +23319,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B79" t="s">
         <v>717</v>
@@ -23336,7 +23330,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B80" t="s">
         <v>580</v>
@@ -23347,7 +23341,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B81" t="s">
         <v>727</v>
@@ -23358,7 +23352,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B82" t="s">
         <v>572</v>
@@ -23369,7 +23363,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B83" t="s">
         <v>598</v>
@@ -23380,7 +23374,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B84" t="s">
         <v>739</v>
@@ -23391,7 +23385,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B85" t="s">
         <v>706</v>
@@ -23402,7 +23396,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B86" t="s">
         <v>721</v>
@@ -23413,7 +23407,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B87" t="s">
         <v>577</v>
@@ -23424,7 +23418,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B88" t="s">
         <v>556</v>
@@ -23435,7 +23429,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B89" t="s">
         <v>571</v>
@@ -23446,7 +23440,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B90" t="s">
         <v>558</v>
@@ -23457,7 +23451,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B91" t="s">
         <v>550</v>
@@ -23468,7 +23462,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B92" t="s">
         <v>631</v>
@@ -23479,7 +23473,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B93" t="s">
         <v>560</v>
@@ -23490,7 +23484,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B94" t="s">
         <v>746</v>
@@ -23501,7 +23495,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B95" t="s">
         <v>560</v>
@@ -23512,7 +23506,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B96" t="s">
         <v>631</v>
@@ -23523,7 +23517,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B97" t="s">
         <v>550</v>
@@ -23534,21 +23528,21 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B98" t="s">
         <v>558</v>
       </c>
       <c r="C98" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B99" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="C99" t="s">
         <v>558</v>
@@ -23556,7 +23550,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B100" t="s">
         <v>558</v>
@@ -23567,7 +23561,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B101" t="s">
         <v>571</v>
@@ -29322,7 +29316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F0F151F-D3C6-B64A-9E9D-4142E5C7E622}">
   <dimension ref="A1:N129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>